<commit_message>
updates for flipped parcels comparison
</commit_message>
<xml_diff>
--- a/Matlab_scripts/localizer_source.xlsx
+++ b/Matlab_scripts/localizer_source.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruimingao/Documents/TripleEvents/TripleEvents/Matlab_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD760AE-A897-B94E-9AE7-6B0297D19FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304EB65D-DB9A-5440-8BC9-18BB65DD4ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{AD80813E-A688-3447-8287-5FFA2CC7A9B2}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" activeTab="2" xr2:uid="{AD80813E-A688-3447-8287-5FFA2CC7A9B2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="bothContrast" sheetId="1" r:id="rId1"/>
+    <sheet name="picLocalized" sheetId="2" r:id="rId2"/>
+    <sheet name="picLocalized_flipped" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="150">
   <si>
     <t>UID</t>
   </si>
@@ -198,6 +200,294 @@
   </si>
   <si>
     <t>EventsRev</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/199_FED_20160711c_3T1_PL2017/firstlevel_events2move_instrsep/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/261_FED_20160523c_3T2_PL2017/firstlevel_events2move_instrsep/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/407_FED_20160804a_3T1_PL2017/firstlevel_events2move_instrsep/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/408_FED_20160711a2_3T1_PL2017/firstlevel_events2move_instrsep/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/409_FED_20160622a_3T1_PL2017/firstlevel_events2move_instrsep/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/410_FED_20160623b_3T2_PL2017/firstlevel_events2move_instrsep/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/730_FED_20190306a_3T2_PL2017/firstlevel_events2move_instrsep/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/776_FED_20190611b_3T2_PL2017/firstlevel_events2move_instrsep/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/291_FED_20160803c_3T1_PL2017/firstlevel_events2move_instrsep/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/400_FED_20160520a_3T1_PL2017/firstlevel_events2move_instrsep/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/419_FED_20160805a_3T1_PL2017/firstlevel_events2move_instrsep/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/773_FED_20190605c_3T2_PL2017/firstlevel_events2move_instrsep/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/774_FED_20190605b_3T2_PL2017/firstlevel_events2move_instrsep/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/775_FED_20190611a_3T2_PL2017/firstlevel_events2move_instrsep/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/778_FED_20190614b_3T2_PL2017/firstlevel_events2move_instrsep/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/040_KAN_langevents_01_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/057_KAN_langevents_02_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/059_KAN_langevents_04_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/056_KAN_langevents_05_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/067_KAN_langevents_06_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/068_KAN_langevents_07_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/019_KAN_langevents_08_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/070_KAN_langevents_11_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/087_KAN_langevents_12_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/078_KAN_langevents_13_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/089_KAN_langevents_15_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/076_KAN_langevents_16_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_0019_percentile-ROI-levfc45f86d59d40662d392eabea2853563.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/249_FED_20160519a_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/252_FED_20160907b_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/291_FED_20160803c_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/301_FED_20160908b_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/376_FED_20160519b_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/399_FED_20160519d_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/400_FED_20160520a_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/401_FED_20160520d_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/419_FED_20160805a_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/420_FED_20160805b_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/426_FED_20160908d_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/682_FED_20190426a_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/767_FED_20190418b_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/768_FED_20190517a_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/769_FED_20190522a_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/770_FED_20190523b_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/773_FED_20190605c_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/774_FED_20190605b_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/775_FED_20190611a_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/778_FED_20190614b_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/863_FED_20211124a_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_0013_percentile-ROI-lev8b22f9922f761245e20b055b1f57efb8.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/291_FED_20160803c_3T1_PL2017/firstlevel_events2move_instrsep/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/400_FED_20160520a_3T1_PL2017/firstlevel_events2move_instrsep/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/419_FED_20160805a_3T1_PL2017/firstlevel_events2move_instrsep/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/773_FED_20190605c_3T2_PL2017/firstlevel_events2move_instrsep/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/774_FED_20190605b_3T2_PL2017/firstlevel_events2move_instrsep/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/775_FED_20190611a_3T2_PL2017/firstlevel_events2move_instrsep/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/778_FED_20190614b_3T2_PL2017/firstlevel_events2move_instrsep/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/199_FED_20160711c_3T1_PL2017/firstlevel_events2move_instrsep/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/261_FED_20160523c_3T2_PL2017/firstlevel_events2move_instrsep/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/407_FED_20160804a_3T1_PL2017/firstlevel_events2move_instrsep/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/408_FED_20160711a2_3T1_PL2017/firstlevel_events2move_instrsep/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/409_FED_20160622a_3T1_PL2017/firstlevel_events2move_instrsep/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/410_FED_20160623b_3T2_PL2017/firstlevel_events2move_instrsep/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/730_FED_20190306a_3T2_PL2017/firstlevel_events2move_instrsep/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/776_FED_20190611b_3T2_PL2017/firstlevel_events2move_instrsep/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/040_KAN_langevents_01_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/057_KAN_langevents_02_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/059_KAN_langevents_04_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/056_KAN_langevents_05_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/067_KAN_langevents_06_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/068_KAN_langevents_07_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/019_KAN_langevents_08_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/070_KAN_langevents_11_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/087_KAN_langevents_12_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/078_KAN_langevents_13_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/089_KAN_langevents_15_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/076_KAN_langevents_16_PL2017/firstlevel_EventsOrig_instrsep_2runs/locT_conjunction_0020_percenc794b15b1bc19586da8fdcf87e59f700.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/249_FED_20160519a_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/252_FED_20160907b_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/291_FED_20160803c_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/301_FED_20160908b_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/376_FED_20160519b_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/399_FED_20160519d_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/400_FED_20160520a_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/401_FED_20160520d_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/419_FED_20160805a_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/420_FED_20160805b_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/426_FED_20160908d_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/682_FED_20190426a_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/767_FED_20190418b_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/769_FED_20190522a_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/770_FED_20190523b_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/773_FED_20190605c_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/774_FED_20190605b_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/775_FED_20190611a_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/778_FED_20190614b_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/863_FED_20211124a_3T1_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
+  </si>
+  <si>
+    <t>/mindhive/evlab/u/Shared/SUBJECTS/768_FED_20190517a_3T2_PL2017/firstlevel_EventsRev_instrsep/locT_conjunction_0014_percenb2141d8d9d5a6c30246186e03ba1fa0c.nii</t>
   </si>
 </sst>
 </file>
@@ -579,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9244ABE8-560B-2A41-B30C-415E246028A7}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1127,4 +1417,1112 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4DEB975-ADED-3F46-9EF0-5DBEB0A91837}">
+  <dimension ref="A1:C49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>199</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>261</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>407</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>408</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>409</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <v>410</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>730</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>776</v>
+      </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>291</v>
+      </c>
+      <c r="C10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11">
+        <v>400</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <v>419</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>773</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>774</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <v>775</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>778</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <v>70</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <v>87</v>
+      </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>76</v>
+      </c>
+      <c r="C28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29">
+        <v>249</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30">
+        <v>252</v>
+      </c>
+      <c r="C30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31">
+        <v>291</v>
+      </c>
+      <c r="C31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32">
+        <v>301</v>
+      </c>
+      <c r="C32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33">
+        <v>376</v>
+      </c>
+      <c r="C33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34">
+        <v>399</v>
+      </c>
+      <c r="C34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35">
+        <v>400</v>
+      </c>
+      <c r="C35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36">
+        <v>401</v>
+      </c>
+      <c r="C36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37">
+        <v>419</v>
+      </c>
+      <c r="C37" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38">
+        <v>420</v>
+      </c>
+      <c r="C38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39">
+        <v>426</v>
+      </c>
+      <c r="C39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40">
+        <v>682</v>
+      </c>
+      <c r="C40" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41">
+        <v>767</v>
+      </c>
+      <c r="C41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42">
+        <v>768</v>
+      </c>
+      <c r="C42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43">
+        <v>769</v>
+      </c>
+      <c r="C43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44">
+        <v>770</v>
+      </c>
+      <c r="C44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45">
+        <v>773</v>
+      </c>
+      <c r="C45" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46">
+        <v>774</v>
+      </c>
+      <c r="C46" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47">
+        <v>775</v>
+      </c>
+      <c r="C47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48">
+        <v>778</v>
+      </c>
+      <c r="C48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49">
+        <v>863</v>
+      </c>
+      <c r="C49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F145BA8-597D-3F4C-B433-39A8328D0817}">
+  <dimension ref="A1:C49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>199</v>
+      </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>261</v>
+      </c>
+      <c r="C3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>407</v>
+      </c>
+      <c r="C4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>408</v>
+      </c>
+      <c r="C5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>409</v>
+      </c>
+      <c r="C6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <v>410</v>
+      </c>
+      <c r="C7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>730</v>
+      </c>
+      <c r="C8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>776</v>
+      </c>
+      <c r="C9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>291</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11">
+        <v>400</v>
+      </c>
+      <c r="C11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <v>419</v>
+      </c>
+      <c r="C12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>773</v>
+      </c>
+      <c r="C13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>774</v>
+      </c>
+      <c r="C14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <v>775</v>
+      </c>
+      <c r="C15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>778</v>
+      </c>
+      <c r="C16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <v>70</v>
+      </c>
+      <c r="C24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <v>87</v>
+      </c>
+      <c r="C25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>76</v>
+      </c>
+      <c r="C28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29">
+        <v>249</v>
+      </c>
+      <c r="C29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30">
+        <v>252</v>
+      </c>
+      <c r="C30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31">
+        <v>291</v>
+      </c>
+      <c r="C31" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32">
+        <v>301</v>
+      </c>
+      <c r="C32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33">
+        <v>376</v>
+      </c>
+      <c r="C33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34">
+        <v>399</v>
+      </c>
+      <c r="C34" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35">
+        <v>400</v>
+      </c>
+      <c r="C35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36">
+        <v>401</v>
+      </c>
+      <c r="C36" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37">
+        <v>419</v>
+      </c>
+      <c r="C37" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38">
+        <v>420</v>
+      </c>
+      <c r="C38" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39">
+        <v>426</v>
+      </c>
+      <c r="C39" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40">
+        <v>682</v>
+      </c>
+      <c r="C40" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41">
+        <v>767</v>
+      </c>
+      <c r="C41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42">
+        <v>768</v>
+      </c>
+      <c r="C42" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43">
+        <v>769</v>
+      </c>
+      <c r="C43" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44">
+        <v>770</v>
+      </c>
+      <c r="C44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45">
+        <v>773</v>
+      </c>
+      <c r="C45" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46">
+        <v>774</v>
+      </c>
+      <c r="C46" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47">
+        <v>775</v>
+      </c>
+      <c r="C47" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48">
+        <v>778</v>
+      </c>
+      <c r="C48" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49">
+        <v>863</v>
+      </c>
+      <c r="C49" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>